<commit_message>
ajustes de colores y pruebas
</commit_message>
<xml_diff>
--- a/chats/593997871569@c.us.xlsx
+++ b/chats/593997871569@c.us.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -77,6 +77,33 @@
   </si>
   <si>
     <t>14-11-2021 11:26</t>
+  </si>
+  <si>
+    <t>15-11-2021 11:18</t>
+  </si>
+  <si>
+    <t>Xexe</t>
+  </si>
+  <si>
+    <t>Fv</t>
+  </si>
+  <si>
+    <t>15-11-2021 12:00</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>15-11-2021 12:51</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>15-11-2021 01:47</t>
+  </si>
+  <si>
+    <t>Xbxjd</t>
   </si>
 </sst>
 </file>
@@ -453,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B18"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -560,6 +587,46 @@
         <v>7</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>